<commit_message>
recursive digit sum edit
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/91940fcd53e0849a/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data-Structures-and-Algorithms-\Data-Structures-and-Algorithms-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="8_{BE793299-5568-40FF-BC42-BD2E7E08F337}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{643A7DAA-85D7-49DB-8509-B4CDBE94C6B4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498AA453-27AD-4C0C-B7A8-AAA9634B7087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C11F6346-89F9-4D0D-A643-96055F000ABB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="566">
   <si>
     <t>Topic</t>
   </si>
@@ -1648,13 +1648,88 @@
   </si>
   <si>
     <t>Using bitmasking above technique was followed</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>Using backtracking, we use a loop to call for all possibilites on the keypad and store them in the answer vector</t>
+  </si>
+  <si>
+    <t>Using a recursion code, we make a boolean returning function which calls only when the condition is true.</t>
+  </si>
+  <si>
+    <t>See tower of hanoi concept</t>
+  </si>
+  <si>
+    <t>Apply simple one line recursion to solve the statement</t>
+  </si>
+  <si>
+    <t>towerOfHanoi</t>
+  </si>
+  <si>
+    <t>recursiveDigitsum</t>
+  </si>
+  <si>
+    <t>fromAtoB</t>
+  </si>
+  <si>
+    <t>keypad</t>
+  </si>
+  <si>
+    <t>subset</t>
+  </si>
+  <si>
+    <t>marvoloGauntRing</t>
+  </si>
+  <si>
+    <t>matrixBlockSum</t>
+  </si>
+  <si>
+    <t>waterLevel</t>
+  </si>
+  <si>
+    <t>chunksInArray</t>
+  </si>
+  <si>
+    <t>clockwiseRotate</t>
+  </si>
+  <si>
+    <t>maxProfit</t>
+  </si>
+  <si>
+    <t>alyonaFlowers</t>
+  </si>
+  <si>
+    <t>minswaps</t>
+  </si>
+  <si>
+    <t>sumOfAllSubarray</t>
+  </si>
+  <si>
+    <t>sumOfAllSubmatrices</t>
+  </si>
+  <si>
+    <t>rangeSumQuery2D</t>
+  </si>
+  <si>
+    <t>searchInSorted2D</t>
+  </si>
+  <si>
+    <t>maxVowelsInsubstr</t>
+  </si>
+  <si>
+    <t>stringPermutations</t>
+  </si>
+  <si>
+    <t>starrySky</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1666,6 +1741,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1692,13 +1775,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2014,10 +2098,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C075FCED-F15A-4BC7-B5F0-A5F1F14A4DA9}">
-  <dimension ref="A1:D500"/>
+  <dimension ref="A1:E500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2026,23 +2110,27 @@
     <col min="2" max="2" width="69.28515625" customWidth="1"/>
     <col min="3" max="3" width="6.7109375" customWidth="1"/>
     <col min="4" max="4" width="152.7109375" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="4" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2055,8 +2143,11 @@
       <c r="D2" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2069,8 +2160,11 @@
       <c r="D3" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2083,8 +2177,11 @@
       <c r="D4" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2097,8 +2194,11 @@
       <c r="D5" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -2111,8 +2211,11 @@
       <c r="D6" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -2125,8 +2228,11 @@
       <c r="D7" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -2139,8 +2245,11 @@
       <c r="D8" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -2153,8 +2262,11 @@
       <c r="D9" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -2167,8 +2279,11 @@
       <c r="D10" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -2181,8 +2296,11 @@
       <c r="D11" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -2195,8 +2313,11 @@
       <c r="D12" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -2209,8 +2330,11 @@
       <c r="D13" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -2223,8 +2347,11 @@
       <c r="D14" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -2237,8 +2364,11 @@
       <c r="D15" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -2251,8 +2381,11 @@
       <c r="D16" t="s">
         <v>536</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -2265,8 +2398,11 @@
       <c r="D17" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -2279,8 +2415,11 @@
       <c r="D18" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -2288,7 +2427,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -2296,7 +2435,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -2304,7 +2443,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -2312,7 +2451,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -2320,7 +2459,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -2328,7 +2467,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -2336,7 +2475,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -2344,7 +2483,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -2352,7 +2491,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -2360,7 +2499,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -2368,7 +2507,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -2376,7 +2515,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2384,7 +2523,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -2392,7 +2531,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -2400,7 +2539,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -2408,7 +2547,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>30</v>
       </c>
@@ -2416,7 +2555,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -2424,7 +2563,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -2432,7 +2571,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>30</v>
       </c>
@@ -2440,7 +2579,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>30</v>
       </c>
@@ -2448,7 +2587,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>30</v>
       </c>
@@ -2456,7 +2595,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>30</v>
       </c>
@@ -2464,7 +2603,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>30</v>
       </c>
@@ -2472,7 +2611,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>30</v>
       </c>
@@ -2480,7 +2619,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -2493,8 +2632,11 @@
       <c r="D44" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -2507,40 +2649,76 @@
       <c r="D45" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>48</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>531</v>
+      </c>
+      <c r="D46" t="s">
+        <v>542</v>
+      </c>
+      <c r="E46" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>48</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>531</v>
+      </c>
+      <c r="D47" t="s">
+        <v>543</v>
+      </c>
+      <c r="E47" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>110</v>
+      </c>
+      <c r="D48" t="s">
+        <v>545</v>
+      </c>
+      <c r="E48" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>110</v>
+      </c>
+      <c r="D49" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -2548,7 +2726,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -2556,7 +2734,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>48</v>
       </c>
@@ -2564,7 +2742,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>48</v>
       </c>
@@ -2572,7 +2750,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -2580,7 +2758,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>48</v>
       </c>
@@ -2588,7 +2766,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>48</v>
       </c>
@@ -2596,7 +2774,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>48</v>
       </c>
@@ -2604,7 +2782,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>48</v>
       </c>
@@ -2612,7 +2790,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>48</v>
       </c>
@@ -2620,7 +2798,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>48</v>
       </c>
@@ -2628,7 +2806,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>48</v>
       </c>
@@ -2636,7 +2814,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>48</v>
       </c>
@@ -2644,7 +2822,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>48</v>
       </c>
@@ -2652,7 +2830,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>69</v>
       </c>

</xml_diff>

<commit_message>
added some more approaches
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data-Structures-and-Algorithms-\Data-Structures-and-Algorithms-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8AA8B60-FD68-48E2-8FED-8E16FB2C33EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027E9035-9086-4FDB-B764-0A5B2F743825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C11F6346-89F9-4D0D-A643-96055F000ABB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="594">
   <si>
     <t>Topic</t>
   </si>
@@ -1789,6 +1789,24 @@
   </si>
   <si>
     <t>largestNumber</t>
+  </si>
+  <si>
+    <t>Iterate on the array while storing the elements in the map check for the difference of the sum and each element in the map, if its found return true else keep the answer false till the end</t>
+  </si>
+  <si>
+    <t>pairSum</t>
+  </si>
+  <si>
+    <t>pairDifference</t>
+  </si>
+  <si>
+    <t>pairSum2</t>
+  </si>
+  <si>
+    <t>if there are repeating elements which makes the sum then using combination formula find the count, apply two pointers after sorting the input array to get the total count</t>
+  </si>
+  <si>
+    <t>in case of diffrence apply both conditions where difference and difference*(-1) after sorting the array and applying the two pointers</t>
   </si>
 </sst>
 </file>
@@ -2166,8 +2184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C075FCED-F15A-4BC7-B5F0-A5F1F14A4DA9}">
   <dimension ref="A1:E500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E106" sqref="E106"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D150" sqref="D150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3682,7 +3700,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
         <v>108</v>
       </c>
@@ -3690,7 +3708,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>108</v>
       </c>
@@ -3701,7 +3719,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
         <v>108</v>
       </c>
@@ -3712,31 +3730,58 @@
         <v>110</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
         <v>157</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C148" t="s">
+        <v>110</v>
+      </c>
+      <c r="D148" t="s">
+        <v>588</v>
+      </c>
+      <c r="E148" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
         <v>157</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C149" t="s">
+        <v>110</v>
+      </c>
+      <c r="D149" t="s">
+        <v>592</v>
+      </c>
+      <c r="E149" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
         <v>157</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C150" t="s">
+        <v>110</v>
+      </c>
+      <c r="D150" t="s">
+        <v>593</v>
+      </c>
+      <c r="E150" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
         <v>157</v>
       </c>
@@ -3744,7 +3789,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
         <v>157</v>
       </c>
@@ -3752,7 +3797,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
         <v>157</v>
       </c>
@@ -3760,7 +3805,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
         <v>157</v>
       </c>
@@ -3768,7 +3813,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
         <v>157</v>
       </c>
@@ -3776,7 +3821,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
         <v>157</v>
       </c>
@@ -3784,7 +3829,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
         <v>157</v>
       </c>
@@ -3792,7 +3837,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
         <v>157</v>
       </c>
@@ -3800,7 +3845,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
         <v>157</v>
       </c>
@@ -3808,7 +3853,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
         <v>157</v>
       </c>

</xml_diff>

<commit_message>
added count pair difference
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data-Structures-and-Algorithms-\Data-Structures-and-Algorithms-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027E9035-9086-4FDB-B764-0A5B2F743825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A022FEC-3929-4DB7-8D8B-EF5EF7A209D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C11F6346-89F9-4D0D-A643-96055F000ABB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1219" uniqueCount="596">
   <si>
     <t>Topic</t>
   </si>
@@ -1807,6 +1807,12 @@
   </si>
   <si>
     <t>in case of diffrence apply both conditions where difference and difference*(-1) after sorting the array and applying the two pointers</t>
+  </si>
+  <si>
+    <t>Make use of a map to store the frequency of all the elements of the map and then find the diffrences of the elements present in the map, calculating all the combinations,sum up for answer</t>
+  </si>
+  <si>
+    <t>coutPairDiff</t>
   </si>
 </sst>
 </file>
@@ -2184,8 +2190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C075FCED-F15A-4BC7-B5F0-A5F1F14A4DA9}">
   <dimension ref="A1:E500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D150" sqref="D150"/>
+    <sheetView tabSelected="1" topLeftCell="C139" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E151" sqref="E151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3787,6 +3793,15 @@
       </c>
       <c r="B151" s="2" t="s">
         <v>160</v>
+      </c>
+      <c r="C151" t="s">
+        <v>110</v>
+      </c>
+      <c r="D151" t="s">
+        <v>594</v>
+      </c>
+      <c r="E151" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added union of two arrays
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data-Structures-and-Algorithms-\Data-Structures-and-Algorithms-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A022FEC-3929-4DB7-8D8B-EF5EF7A209D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185E4022-A755-4153-9979-020554D98E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C11F6346-89F9-4D0D-A643-96055F000ABB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1219" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="597">
   <si>
     <t>Topic</t>
   </si>
@@ -1813,6 +1813,9 @@
   </si>
   <si>
     <t>coutPairDiff</t>
+  </si>
+  <si>
+    <t>Insert in a set or use two pointers one from start of one array and one from end of other array, insert them into a set and convert it into a vector,then sort the vector</t>
   </si>
 </sst>
 </file>
@@ -2190,8 +2193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C075FCED-F15A-4BC7-B5F0-A5F1F14A4DA9}">
   <dimension ref="A1:E500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C139" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E151" sqref="E151"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B152" sqref="B152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3810,6 +3813,12 @@
       </c>
       <c r="B152" s="2" t="s">
         <v>161</v>
+      </c>
+      <c r="C152" t="s">
+        <v>110</v>
+      </c>
+      <c r="D152" t="s">
+        <v>596</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added intersection of 2 arrays efficient code
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data-Structures-and-Algorithms-\Data-Structures-and-Algorithms-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185E4022-A755-4153-9979-020554D98E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44A0A00-22D9-4E30-8EB5-4FE8F3CF9DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C11F6346-89F9-4D0D-A643-96055F000ABB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="600">
   <si>
     <t>Topic</t>
   </si>
@@ -1816,6 +1816,15 @@
   </si>
   <si>
     <t>Insert in a set or use two pointers one from start of one array and one from end of other array, insert them into a set and convert it into a vector,then sort the vector</t>
+  </si>
+  <si>
+    <t>if the arrays are sorted then use 2 pointers in each array to find the intersection in O(n) time complexity and O(1) space complexity.</t>
+  </si>
+  <si>
+    <t>unionOfTwoArrays</t>
+  </si>
+  <si>
+    <t>intersectionOf2Arrays</t>
   </si>
 </sst>
 </file>
@@ -2193,8 +2202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C075FCED-F15A-4BC7-B5F0-A5F1F14A4DA9}">
   <dimension ref="A1:E500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B152" sqref="B152"/>
+    <sheetView tabSelected="1" topLeftCell="C139" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D156" sqref="D156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3820,6 +3829,9 @@
       <c r="D152" t="s">
         <v>596</v>
       </c>
+      <c r="E152" t="s">
+        <v>598</v>
+      </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
@@ -3827,6 +3839,15 @@
       </c>
       <c r="B153" s="1" t="s">
         <v>162</v>
+      </c>
+      <c r="C153" t="s">
+        <v>110</v>
+      </c>
+      <c r="D153" t="s">
+        <v>597</v>
+      </c>
+      <c r="E153" t="s">
+        <v>599</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added power of two in bit manipultaion
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data-Structures-and-Algorithms-\Data-Structures-and-Algorithms-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44A0A00-22D9-4E30-8EB5-4FE8F3CF9DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8108BCFA-3A6D-4E08-8A9D-BA6C5BD121C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C11F6346-89F9-4D0D-A643-96055F000ABB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="602">
   <si>
     <t>Topic</t>
   </si>
@@ -1825,6 +1825,12 @@
   </si>
   <si>
     <t>intersectionOf2Arrays</t>
+  </si>
+  <si>
+    <t>using left shift operator calculate every power of 2 from 1 to 31 and get answer in O(32) time complexity.</t>
+  </si>
+  <si>
+    <t>powerOf2</t>
   </si>
 </sst>
 </file>
@@ -2202,8 +2208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C075FCED-F15A-4BC7-B5F0-A5F1F14A4DA9}">
   <dimension ref="A1:E500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C139" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D156" sqref="D156"/>
+    <sheetView tabSelected="1" topLeftCell="C143" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E173" sqref="E173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3906,7 +3912,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
         <v>157</v>
       </c>
@@ -3914,7 +3920,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
         <v>157</v>
       </c>
@@ -3922,7 +3928,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
         <v>157</v>
       </c>
@@ -3930,7 +3936,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
         <v>157</v>
       </c>
@@ -3938,7 +3944,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
         <v>157</v>
       </c>
@@ -3946,7 +3952,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
         <v>157</v>
       </c>
@@ -3954,7 +3960,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
         <v>157</v>
       </c>
@@ -3962,7 +3968,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
         <v>157</v>
       </c>
@@ -3970,7 +3976,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
         <v>157</v>
       </c>
@@ -3978,7 +3984,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
         <v>157</v>
       </c>
@@ -3986,7 +3992,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
         <v>157</v>
       </c>
@@ -3994,7 +4000,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
         <v>157</v>
       </c>
@@ -4002,7 +4008,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
         <v>182</v>
       </c>
@@ -4012,8 +4018,14 @@
       <c r="C173" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D173" t="s">
+        <v>600</v>
+      </c>
+      <c r="E173" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
         <v>182</v>
       </c>
@@ -4024,7 +4036,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
         <v>182</v>
       </c>
@@ -4035,7 +4047,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
         <v>182</v>
       </c>

</xml_diff>

<commit_message>
added count of 1
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data-Structures-and-Algorithms-\Data-Structures-and-Algorithms-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8108BCFA-3A6D-4E08-8A9D-BA6C5BD121C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1885D4F-8CA1-416F-9497-7F01991FCDCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C11F6346-89F9-4D0D-A643-96055F000ABB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2463" uniqueCount="609">
   <si>
     <t>Topic</t>
   </si>
@@ -1831,6 +1831,27 @@
   </si>
   <si>
     <t>powerOf2</t>
+  </si>
+  <si>
+    <t>use right shift and check if the number is odd then count the occurrence of the odd numbers whenever right shifting, it will the answer</t>
+  </si>
+  <si>
+    <t>use right shift and check if the number is odd then power the occurrence of the odd numbers whenever right shifting, ow will the answer</t>
+  </si>
+  <si>
+    <t>use right shift and check if the number is odd then bleak the occurrence of the odd numbers whenever right shifting, um will the answer</t>
+  </si>
+  <si>
+    <t>use right shift and check if the number is odd then steps the occurrence of the odd numbers whenever right shifting, te will the answer</t>
+  </si>
+  <si>
+    <t>use right shift and check if the number is odd then number the occurrence of the odd numbers whenever right shifting, um will the answer</t>
+  </si>
+  <si>
+    <t>use right shift and check if the number is odd then hamming the occurrence of the odd numbers whenever right shifting, is will the answer</t>
+  </si>
+  <si>
+    <t>countOf1</t>
   </si>
 </sst>
 </file>
@@ -2209,7 +2230,7 @@
   <dimension ref="A1:E500"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C143" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E173" sqref="E173"/>
+      <selection activeCell="E174" sqref="E174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4034,6 +4055,12 @@
       </c>
       <c r="C174" t="s">
         <v>110</v>
+      </c>
+      <c r="D174" t="s">
+        <v>602</v>
+      </c>
+      <c r="E174" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added power of 2 and subsequences
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data-Structures-and-Algorithms-\Data-Structures-and-Algorithms-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data-Structures-and-Algorithms-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1885D4F-8CA1-416F-9497-7F01991FCDCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A15A07-03A5-44F8-9F6A-D5F4BAAA7773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C11F6346-89F9-4D0D-A643-96055F000ABB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2463" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="608">
   <si>
     <t>Topic</t>
   </si>
@@ -1836,22 +1836,19 @@
     <t>use right shift and check if the number is odd then count the occurrence of the odd numbers whenever right shifting, it will the answer</t>
   </si>
   <si>
-    <t>use right shift and check if the number is odd then power the occurrence of the odd numbers whenever right shifting, ow will the answer</t>
-  </si>
-  <si>
-    <t>use right shift and check if the number is odd then bleak the occurrence of the odd numbers whenever right shifting, um will the answer</t>
-  </si>
-  <si>
-    <t>use right shift and check if the number is odd then steps the occurrence of the odd numbers whenever right shifting, te will the answer</t>
-  </si>
-  <si>
-    <t>use right shift and check if the number is odd then number the occurrence of the odd numbers whenever right shifting, um will the answer</t>
-  </si>
-  <si>
-    <t>use right shift and check if the number is odd then hamming the occurrence of the odd numbers whenever right shifting, is will the answer</t>
-  </si>
-  <si>
     <t>countOf1</t>
+  </si>
+  <si>
+    <t>check for the most significant bit of both numbers, while shifting the mask number(1L&lt;&lt;31) to the right, check whenever the MSB of both left and right is 1 using mask,add mask to the answer</t>
+  </si>
+  <si>
+    <t>bitwise_and_in_range</t>
+  </si>
+  <si>
+    <t>first check for each number if it’s a power of 2 by using if((num&amp;num-1)==0), then count the number of power of 2, believe those counts as a new array, and total subsequences = 2^N -1</t>
+  </si>
+  <si>
+    <t>powerOf2AndSubseq</t>
   </si>
 </sst>
 </file>
@@ -2230,7 +2227,7 @@
   <dimension ref="A1:E500"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C143" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E174" sqref="E174"/>
+      <selection activeCell="E176" sqref="E176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4060,7 +4057,7 @@
         <v>602</v>
       </c>
       <c r="E174" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
@@ -4073,6 +4070,12 @@
       <c r="C175" t="s">
         <v>110</v>
       </c>
+      <c r="D175" t="s">
+        <v>604</v>
+      </c>
+      <c r="E175" t="s">
+        <v>605</v>
+      </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
@@ -4080,6 +4083,15 @@
       </c>
       <c r="B176" s="1" t="s">
         <v>186</v>
+      </c>
+      <c r="C176" t="s">
+        <v>110</v>
+      </c>
+      <c r="D176" t="s">
+        <v>606</v>
+      </c>
+      <c r="E176" t="s">
+        <v>607</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added binary search over answer concept
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data-Structures-and-Algorithms-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9948D591-B8B4-4DDD-B2AB-E6FF80A776EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD43605-3111-4183-9093-A29C033F71CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C11F6346-89F9-4D0D-A643-96055F000ABB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="617">
   <si>
     <t>Topic</t>
   </si>
@@ -1864,6 +1864,18 @@
   </si>
   <si>
     <t>do xor for all elements in the array,the number occuring once will not be cancelled out while rest fo the elements occurring more than once will cancel out each other</t>
+  </si>
+  <si>
+    <t>use a basice hash map with element as index and its its index as the storing value, check for x-arr[i] in the map and make sure its not the same element as arr[i]</t>
+  </si>
+  <si>
+    <t>set_pair</t>
+  </si>
+  <si>
+    <t>subarray_sum_0</t>
+  </si>
+  <si>
+    <t>take premax of the array and store its frequency in map, iterate the map and find any element with freq more than 1 return true, or if the map is empty return true</t>
   </si>
 </sst>
 </file>
@@ -2241,8 +2253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C075FCED-F15A-4BC7-B5F0-A5F1F14A4DA9}">
   <dimension ref="A1:E500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D152" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E179" sqref="E179"/>
+    <sheetView tabSelected="1" topLeftCell="A179" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D194" sqref="D194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4276,7 +4288,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="s">
         <v>203</v>
       </c>
@@ -4286,8 +4298,14 @@
       <c r="C193" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D193" t="s">
+        <v>613</v>
+      </c>
+      <c r="E193" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
         <v>203</v>
       </c>
@@ -4297,8 +4315,14 @@
       <c r="C194" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D194" t="s">
+        <v>616</v>
+      </c>
+      <c r="E194" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
         <v>203</v>
       </c>
@@ -4309,7 +4333,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="3" t="s">
         <v>203</v>
       </c>
@@ -4320,7 +4344,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="s">
         <v>203</v>
       </c>
@@ -4328,7 +4352,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="3" t="s">
         <v>203</v>
       </c>
@@ -4336,7 +4360,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="3" t="s">
         <v>203</v>
       </c>
@@ -4344,7 +4368,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="3" t="s">
         <v>203</v>
       </c>
@@ -4352,7 +4376,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="3" t="s">
         <v>203</v>
       </c>
@@ -4360,7 +4384,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="3" t="s">
         <v>203</v>
       </c>
@@ -4371,7 +4395,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="3" t="s">
         <v>203</v>
       </c>
@@ -4382,7 +4406,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="3" t="s">
         <v>203</v>
       </c>
@@ -4390,7 +4414,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="3" t="s">
         <v>203</v>
       </c>
@@ -4398,7 +4422,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="s">
         <v>203</v>
       </c>
@@ -4406,7 +4430,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
         <v>203</v>
       </c>
@@ -4417,7 +4441,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" s="3" t="s">
         <v>203</v>
       </c>

</xml_diff>

<commit_message>
added radix sort and qualifying contest
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data-Structures-and-Algorithms-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD43605-3111-4183-9093-A29C033F71CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE40ED6C-7151-4573-B8F7-B8CF94BFC776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C11F6346-89F9-4D0D-A643-96055F000ABB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="618">
   <si>
     <t>Topic</t>
   </si>
@@ -1876,6 +1876,9 @@
   </si>
   <si>
     <t>take premax of the array and store its frequency in map, iterate the map and find any element with freq more than 1 return true, or if the map is empty return true</t>
+  </si>
+  <si>
+    <t>Start with the top right element of the matrix and then decrement cloumns till you reach 0 then increment the row and store the row no. as the current answer, iterate till the last row</t>
   </si>
 </sst>
 </file>
@@ -2253,8 +2256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C075FCED-F15A-4BC7-B5F0-A5F1F14A4DA9}">
   <dimension ref="A1:E500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A179" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D194" sqref="D194"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2578,6 +2581,12 @@
       </c>
       <c r="B19" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="C19" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" t="s">
+        <v>617</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added countPrimes and maximizeTheConfusionOfExam
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data-Structures-and-Algorithms-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE40ED6C-7151-4573-B8F7-B8CF94BFC776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F4E478-EE70-4B1D-BB3A-9EE88C6D1F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C11F6346-89F9-4D0D-A643-96055F000ABB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="618">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1253" uniqueCount="621">
   <si>
     <t>Topic</t>
   </si>
@@ -1879,6 +1879,15 @@
   </si>
   <si>
     <t>Start with the top right element of the matrix and then decrement cloumns till you reach 0 then increment the row and store the row no. as the current answer, iterate till the last row</t>
+  </si>
+  <si>
+    <t>Using Sieve of Eratosthenes</t>
+  </si>
+  <si>
+    <t>Maximize the Confusion of an Exam - LeetCode</t>
+  </si>
+  <si>
+    <t>Using binary search on answer and use sliding window on helper function</t>
   </si>
 </sst>
 </file>
@@ -2254,10 +2263,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C075FCED-F15A-4BC7-B5F0-A5F1F14A4DA9}">
-  <dimension ref="A1:E500"/>
+  <dimension ref="A1:E501"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A484" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D501" sqref="D501"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2724,6 +2733,12 @@
       <c r="B36" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="C36" t="s">
+        <v>110</v>
+      </c>
+      <c r="D36" t="s">
+        <v>618</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -6978,7 +6993,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="497" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A497" s="3" t="s">
         <v>473</v>
       </c>
@@ -6986,7 +7001,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="498" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A498" s="3" t="s">
         <v>473</v>
       </c>
@@ -6994,7 +7009,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="499" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A499" s="3" t="s">
         <v>473</v>
       </c>
@@ -7002,12 +7017,26 @@
         <v>518</v>
       </c>
     </row>
-    <row r="500" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A500" s="3" t="s">
         <v>473</v>
       </c>
       <c r="B500" s="1" t="s">
         <v>519</v>
+      </c>
+    </row>
+    <row r="501" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A501" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B501" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="C501" t="s">
+        <v>110</v>
+      </c>
+      <c r="D501" t="s">
+        <v>620</v>
       </c>
     </row>
   </sheetData>
@@ -7511,8 +7540,9 @@
     <hyperlink ref="B498" r:id="rId497" display="https://leetcode.com/problems/unique-paths-ii/" xr:uid="{B9E6644B-53C2-4BD8-889C-E506181EF24E}"/>
     <hyperlink ref="B499" r:id="rId498" display="https://leetcode.com/problems/minimum-path-sum/" xr:uid="{E0370F32-402A-42D5-8187-2C0905CD2C4A}"/>
     <hyperlink ref="B500" r:id="rId499" display="https://leetcode.com/problems/minimum-path-sum/" xr:uid="{E95D9DC6-2693-405A-B852-0AFDD7936DC1}"/>
+    <hyperlink ref="B501" r:id="rId500" display="https://leetcode.com/problems/maximize-the-confusion-of-an-exam/" xr:uid="{79E5386B-DE2B-4F5A-95AE-CC2D428E1228}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId500"/>
+  <pageSetup orientation="portrait" r:id="rId501"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
addition of leetcode question bank
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data-Structures-and-Algorithms-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F4E478-EE70-4B1D-BB3A-9EE88C6D1F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE13333-8F3B-461A-B280-5757F626F712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C11F6346-89F9-4D0D-A643-96055F000ABB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1253" uniqueCount="621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1269" uniqueCount="628">
   <si>
     <t>Topic</t>
   </si>
@@ -1888,6 +1888,27 @@
   </si>
   <si>
     <t>Using binary search on answer and use sliding window on helper function</t>
+  </si>
+  <si>
+    <t>from the question you can derieve that it asks to print 1 if the hcf of all elements is 1 else 0</t>
+  </si>
+  <si>
+    <t>Use recursion to traverse and count the path only if it reaches the destnation and return sum of counts</t>
+  </si>
+  <si>
+    <t>Set Matrix Zeroes - LeetCode</t>
+  </si>
+  <si>
+    <t>Use the same matrix by marking the first elment in both row and col whenever encountering 0 in any arr[row][col] and look out for the corner case at arr[0][0]=0</t>
+  </si>
+  <si>
+    <t>Product of Array Except Self - LeetCode</t>
+  </si>
+  <si>
+    <t>Using prefix product and suffix product</t>
+  </si>
+  <si>
+    <t>Find the Smallest Divisor Given a Threshold - LeetCode</t>
   </si>
 </sst>
 </file>
@@ -2263,10 +2284,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C075FCED-F15A-4BC7-B5F0-A5F1F14A4DA9}">
-  <dimension ref="A1:E501"/>
+  <dimension ref="A1:E504"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A484" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D501" sqref="D501"/>
+    <sheetView tabSelected="1" topLeftCell="A480" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B501" sqref="B501"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2693,6 +2714,12 @@
       <c r="B31" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="C31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" t="s">
+        <v>621</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -2905,6 +2932,12 @@
       <c r="B50" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="C50" t="s">
+        <v>531</v>
+      </c>
+      <c r="D50" t="s">
+        <v>622</v>
+      </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -7036,6 +7069,48 @@
         <v>110</v>
       </c>
       <c r="D501" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="502" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A502" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B502" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="C502" t="s">
+        <v>110</v>
+      </c>
+      <c r="D502" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="503" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A503" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B503" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="C503" t="s">
+        <v>110</v>
+      </c>
+      <c r="D503" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="504" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A504" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B504" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="C504" t="s">
+        <v>110</v>
+      </c>
+      <c r="D504" t="s">
         <v>620</v>
       </c>
     </row>
@@ -7541,8 +7616,11 @@
     <hyperlink ref="B499" r:id="rId498" display="https://leetcode.com/problems/minimum-path-sum/" xr:uid="{E0370F32-402A-42D5-8187-2C0905CD2C4A}"/>
     <hyperlink ref="B500" r:id="rId499" display="https://leetcode.com/problems/minimum-path-sum/" xr:uid="{E95D9DC6-2693-405A-B852-0AFDD7936DC1}"/>
     <hyperlink ref="B501" r:id="rId500" display="https://leetcode.com/problems/maximize-the-confusion-of-an-exam/" xr:uid="{79E5386B-DE2B-4F5A-95AE-CC2D428E1228}"/>
+    <hyperlink ref="B502" r:id="rId501" display="https://leetcode.com/problems/set-matrix-zeroes/" xr:uid="{6CD30627-B2BA-43DB-B3DB-C83DDC694806}"/>
+    <hyperlink ref="B503" r:id="rId502" display="https://leetcode.com/problems/product-of-array-except-self/" xr:uid="{46DAD3A1-DB9B-42BD-A8B5-C983F58C8555}"/>
+    <hyperlink ref="B504" r:id="rId503" display="https://leetcode.com/problems/find-the-smallest-divisor-given-a-threshold/" xr:uid="{B3B80ACA-A4C5-43F2-B0CB-4A440FF234CB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId501"/>
+  <pageSetup orientation="portrait" r:id="rId504"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
WA split3 new changes
</commit_message>
<xml_diff>
--- a/QuestionList.xlsx
+++ b/QuestionList.xlsx
@@ -8,24 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data-Structures-and-Algorithms-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4B268C-37A8-42FD-BECC-DB608CD9890F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C46E17-6284-49D4-AEFA-85FA75FF8D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C11F6346-89F9-4D0D-A643-96055F000ABB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C11F6346-89F9-4D0D-A643-96055F000ABB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1269" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="637">
   <si>
     <t>Topic</t>
   </si>
@@ -1909,6 +1919,33 @@
   </si>
   <si>
     <t>Find the Smallest Divisor Given a Threshold - LeetCode</t>
+  </si>
+  <si>
+    <t>LCM of two consecutive numbers Is 1 and if the number is odd then all n*(n-1)*(n-2) is answer if its even then if its divisible by 3 then (n-1)*(n-2)*(n-3) is ans else n*(n-1)*(n-3) is ans</t>
+  </si>
+  <si>
+    <t>same as array rearrangement but this time modified visited element as a[idx] = a[idx] + a.size()</t>
+  </si>
+  <si>
+    <t>using bucketing to find mix and max elements in each bucket and then finding the answer by subtracting max of bucket with min of successor bucket</t>
+  </si>
+  <si>
+    <t>modify the visited element inside  the array and then calculate answer</t>
+  </si>
+  <si>
+    <t>since the missing element would always be less than size of array, rearrange the array for each element i store it in i-1 idx and iterate on the same indices to find the first missing +ve element</t>
+  </si>
+  <si>
+    <t>use moore voting algorithm</t>
+  </si>
+  <si>
+    <t>use moore voting algorithm after modifying it according to required needs</t>
+  </si>
+  <si>
+    <t>follow simple formula for pascal triangle to fill up the matrix</t>
+  </si>
+  <si>
+    <t>use simple burter force (implementation heavy)</t>
   </si>
 </sst>
 </file>
@@ -2286,8 +2323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C075FCED-F15A-4BC7-B5F0-A5F1F14A4DA9}">
   <dimension ref="A1:E504"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2626,6 +2663,12 @@
       <c r="B20" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="C20" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" t="s">
+        <v>630</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -2634,6 +2677,12 @@
       <c r="B21" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="C21" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21" t="s">
+        <v>631</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -2642,6 +2691,12 @@
       <c r="B22" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="C22" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" t="s">
+        <v>629</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -2650,6 +2705,12 @@
       <c r="B23" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="C23" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" t="s">
+        <v>632</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -2658,6 +2719,12 @@
       <c r="B24" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="C24" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" t="s">
+        <v>633</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -2666,6 +2733,12 @@
       <c r="B25" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="C25" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" t="s">
+        <v>634</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -2674,6 +2747,12 @@
       <c r="B26" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="C26" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" t="s">
+        <v>635</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -2682,6 +2761,12 @@
       <c r="B27" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="C27" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" t="s">
+        <v>636</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -2705,6 +2790,12 @@
       </c>
       <c r="B30" s="2" t="s">
         <v>33</v>
+      </c>
+      <c r="C30" t="s">
+        <v>110</v>
+      </c>
+      <c r="D30" t="s">
+        <v>628</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>